<commit_message>
Total Filed Cases, Related Cases, Not Litigated
</commit_message>
<xml_diff>
--- a/Cases in Film_Music_Arts - List Foundations.xlsx
+++ b/Cases in Film_Music_Arts - List Foundations.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Actresses\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB027B17-DBB3-4113-ACF7-94DBEB71A0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Filed Cases" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Related Cases" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Not Litigated" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Similar" sheetId="4" r:id="rId7"/>
+    <sheet name="Filed Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Related Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Not Litigated" sheetId="3" r:id="rId3"/>
+    <sheet name="Similar" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="725">
   <si>
     <t>State</t>
   </si>
@@ -599,18 +608,24 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">Alki David, </t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t>FilmOn.tv</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>, Hologram USA</t>
     </r>
   </si>
@@ -1257,9 +1272,6 @@
     <t>Criminal</t>
   </si>
   <si>
-    <t>Many-National</t>
-  </si>
-  <si>
     <t>Film, Hollywood</t>
   </si>
   <si>
@@ -1272,9 +1284,6 @@
     <t>https://www.vanityfair.com/hollywood/2003/04/robert-harrison-confidential-magazine</t>
   </si>
   <si>
-    <t>Many- National</t>
-  </si>
-  <si>
     <t>Film, Business</t>
   </si>
   <si>
@@ -2170,43 +2179,96 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Joe_Biden_sexual_assault_allegation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Farmer, Annie Farmer,  Graydon Carter, Vanity Fair Office </t>
+  </si>
+  <si>
+    <t>1996-Present</t>
+  </si>
+  <si>
+    <t>Artist, Art Advisor, Artist-In-Residence, New York Art World, New York Academy of Art</t>
+  </si>
+  <si>
+    <t>Ohio, New York, New Mexico</t>
+  </si>
+  <si>
+    <t>Maria Farmer, Annie Farmer, FBI, New York City Police Department</t>
+  </si>
+  <si>
+    <t>Jeffrey Epstein, Ghislaine Maxwell, Others Unknown</t>
+  </si>
+  <si>
+    <t>Intimidation, Sexual Assault, Harassment, Art Theft</t>
+  </si>
+  <si>
+    <t>Intimidation Interstate, Manipulation and Intimidation of Journalists, Across States, Interstate Threats</t>
+  </si>
+  <si>
+    <t>"In January 2020, Farmer was reportedly working on a series of paintings and pastel drawings called “The Survivors Project” consisting of individual portraits of known survivors of Epstein's abuse," Art</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Maria_Farmer</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2019/08/26/us/epstein-farmer-sisters-maxwell.html</t>
+  </si>
+  <si>
+    <t>Many-National, Hollywood</t>
+  </si>
+  <si>
+    <t>Many- National, Hollywood, Arts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -2215,7 +2277,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2225,74 +2287,46 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -2482,30 +2516,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.38"/>
-    <col customWidth="1" min="2" max="2" width="5.5"/>
-    <col customWidth="1" min="3" max="3" width="15.38"/>
-    <col customWidth="1" min="4" max="4" width="17.38"/>
-    <col customWidth="1" min="6" max="6" width="15.75"/>
-    <col customWidth="1" min="7" max="7" width="15.5"/>
-    <col customWidth="1" min="8" max="8" width="17.63"/>
-    <col customWidth="1" min="9" max="9" width="17.88"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2570,12 +2607,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="1">
-        <v>1937.0</v>
+        <v>1937</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -2611,12 +2648,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1">
-        <v>1954.0</v>
+        <v>1954</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
@@ -2646,12 +2683,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1">
-        <v>2011.0</v>
+        <v>2011</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>41</v>
@@ -2689,12 +2726,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>53</v>
@@ -2730,12 +2767,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1">
-        <v>1997.0</v>
+        <v>1997</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>64</v>
@@ -2763,12 +2800,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B7" s="1">
-        <v>2006.0</v>
+        <v>2006</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>73</v>
@@ -2801,12 +2838,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>82</v>
@@ -2823,8 +2860,8 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
       <c r="T8" s="2" t="s">
         <v>86</v>
       </c>
@@ -2832,12 +2869,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="1">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>88</v>
@@ -2869,17 +2906,17 @@
       <c r="V9" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="W9" s="3"/>
+      <c r="W9" s="1"/>
       <c r="X9" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>100</v>
@@ -2905,14 +2942,14 @@
       <c r="U10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="Z10" s="3"/>
-    </row>
-    <row r="11">
+      <c r="Z10" s="1"/>
+    </row>
+    <row r="11" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>108</v>
@@ -2939,12 +2976,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>116</v>
@@ -2974,12 +3011,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>124</v>
@@ -3003,14 +3040,14 @@
       <c r="K13" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="V13" s="3"/>
-    </row>
-    <row r="14">
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>130</v>
@@ -3027,7 +3064,7 @@
       <c r="I14" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="S14" s="3"/>
+      <c r="S14" s="1"/>
       <c r="T14" s="2" t="s">
         <v>135</v>
       </c>
@@ -3038,12 +3075,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>138</v>
@@ -3065,24 +3102,24 @@
       <c r="K15" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="R15" s="3" t="s">
+      <c r="R15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="4" t="s">
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="3" t="s">
         <v>145</v>
       </c>
       <c r="V15" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B16" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>148</v>
@@ -3110,12 +3147,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>154</v>
@@ -3144,7 +3181,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -3165,8 +3202,8 @@
       </c>
       <c r="I18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
       <c r="T18" s="2" t="s">
         <v>165</v>
       </c>
@@ -3180,7 +3217,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>169</v>
       </c>
@@ -3191,12 +3228,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>172</v>
@@ -3212,8 +3249,8 @@
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
       <c r="T20" s="2" t="s">
         <v>176</v>
       </c>
@@ -3221,12 +3258,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>178</v>
@@ -3243,12 +3280,12 @@
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>182</v>
@@ -3268,8 +3305,8 @@
       <c r="J22" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
       <c r="T22" s="2" t="s">
         <v>187</v>
       </c>
@@ -3277,12 +3314,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>108</v>
@@ -3305,12 +3342,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="1">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>194</v>
@@ -3331,12 +3368,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>199</v>
@@ -3360,7 +3397,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -3383,12 +3420,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>210</v>
@@ -3408,12 +3445,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>214</v>
@@ -3440,12 +3477,12 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>222</v>
@@ -3470,12 +3507,12 @@
         <v>227</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B30" s="1">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>228</v>
@@ -3502,7 +3539,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
@@ -3525,16 +3562,16 @@
       <c r="J31" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-    </row>
-    <row r="32">
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+    </row>
+    <row r="32" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>240</v>
@@ -3554,19 +3591,19 @@
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
       <c r="U32" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="1">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>245</v>
@@ -3588,19 +3625,19 @@
         <v>249</v>
       </c>
       <c r="K33" s="1"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
       <c r="U33" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>251</v>
@@ -3611,13 +3648,13 @@
       <c r="E34" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="1" t="s">
         <v>254</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H34" s="1" t="s">
         <v>256</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -3635,7 +3672,7 @@
       <c r="V34" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="W34" s="3"/>
+      <c r="W34" s="1"/>
       <c r="X34" s="2" t="s">
         <v>260</v>
       </c>
@@ -3646,12 +3683,12 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>263</v>
@@ -3675,12 +3712,12 @@
       <c r="K35" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="W35" s="3"/>
-    </row>
-    <row r="36">
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="W35" s="1"/>
+    </row>
+    <row r="36" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>270</v>
       </c>
@@ -3699,11 +3736,11 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-    </row>
-    <row r="37">
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+    </row>
+    <row r="37" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -3720,7 +3757,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
         <v>279</v>
       </c>
@@ -3742,18 +3779,18 @@
       <c r="K38" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
       <c r="T38" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B39" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>285</v>
@@ -3783,7 +3820,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
@@ -3803,7 +3840,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
@@ -3825,13 +3862,13 @@
       <c r="J41" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
       <c r="T41" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
@@ -3854,7 +3891,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>32</v>
       </c>
@@ -3874,7 +3911,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C44" s="1" t="s">
         <v>307</v>
       </c>
@@ -3885,7 +3922,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
@@ -3908,7 +3945,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
@@ -3928,12 +3965,12 @@
         <v>319</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B47" s="1">
-        <v>1990.0</v>
+        <v>1990</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>320</v>
@@ -3954,7 +3991,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>324</v>
       </c>
@@ -3972,12 +4009,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B49" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>326</v>
@@ -4004,7 +4041,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>21</v>
       </c>
@@ -4027,7 +4064,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>334</v>
       </c>
@@ -4044,7 +4081,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="52" ht="15.0" customHeight="1">
+    <row r="52" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>339</v>
       </c>
@@ -4070,7 +4107,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>21</v>
       </c>
@@ -4099,14 +4136,14 @@
       <c r="V53" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="W53" s="3"/>
-    </row>
-    <row r="54">
+      <c r="W53" s="1"/>
+    </row>
+    <row r="54" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B54" s="1">
-        <v>1943.0</v>
+        <v>1943</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>352</v>
@@ -4124,14 +4161,14 @@
       <c r="J54" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R54" s="3"/>
-      <c r="S54" s="3"/>
-      <c r="T54" s="3"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
       <c r="U54" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>21</v>
       </c>
@@ -4157,12 +4194,12 @@
         <v>359</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B56" s="1">
-        <v>2001.0</v>
+        <v>2001</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>360</v>
@@ -4180,7 +4217,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>21</v>
       </c>
@@ -4204,12 +4241,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B58" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>368</v>
@@ -4239,12 +4276,12 @@
         <v>376</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B59" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>377</v>
@@ -4274,12 +4311,12 @@
         <v>382</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B60" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>383</v>
@@ -4309,12 +4346,12 @@
         <v>388</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B61" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>251</v>
@@ -4340,91 +4377,94 @@
       <c r="R61" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="U61" s="4" t="s">
+      <c r="U61" s="3" t="s">
         <v>393</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2"/>
-    <hyperlink r:id="rId2" ref="U4"/>
-    <hyperlink r:id="rId3" ref="V4"/>
-    <hyperlink r:id="rId4" ref="U6"/>
-    <hyperlink r:id="rId5" ref="U7"/>
-    <hyperlink r:id="rId6" ref="V7"/>
-    <hyperlink r:id="rId7" ref="T8"/>
-    <hyperlink r:id="rId8" ref="U8"/>
-    <hyperlink r:id="rId9" ref="T9"/>
-    <hyperlink r:id="rId10" ref="U9"/>
-    <hyperlink r:id="rId11" ref="V9"/>
-    <hyperlink r:id="rId12" ref="X9"/>
-    <hyperlink r:id="rId13" ref="U10"/>
-    <hyperlink r:id="rId14" ref="U11"/>
-    <hyperlink r:id="rId15" ref="V11"/>
-    <hyperlink r:id="rId16" ref="T12"/>
-    <hyperlink r:id="rId17" ref="U12"/>
-    <hyperlink r:id="rId18" ref="T14"/>
-    <hyperlink r:id="rId19" ref="U14"/>
-    <hyperlink r:id="rId20" ref="V14"/>
-    <hyperlink r:id="rId21" ref="U15"/>
-    <hyperlink r:id="rId22" ref="V15"/>
-    <hyperlink r:id="rId23" ref="T16"/>
-    <hyperlink r:id="rId24" ref="T18"/>
-    <hyperlink r:id="rId25" ref="U18"/>
-    <hyperlink r:id="rId26" ref="V18"/>
-    <hyperlink r:id="rId27" ref="W18"/>
-    <hyperlink r:id="rId28" ref="T20"/>
-    <hyperlink r:id="rId29" ref="U20"/>
-    <hyperlink r:id="rId30" ref="T22"/>
-    <hyperlink r:id="rId31" ref="U22"/>
-    <hyperlink r:id="rId32" ref="U23"/>
-    <hyperlink r:id="rId33" ref="V23"/>
-    <hyperlink r:id="rId34" ref="C24"/>
-    <hyperlink r:id="rId35" ref="U25"/>
-    <hyperlink r:id="rId36" ref="U27"/>
-    <hyperlink r:id="rId37" ref="U28"/>
-    <hyperlink r:id="rId38" ref="U29"/>
-    <hyperlink r:id="rId39" ref="U32"/>
-    <hyperlink r:id="rId40" ref="U33"/>
-    <hyperlink r:id="rId41" ref="U34"/>
-    <hyperlink r:id="rId42" ref="V34"/>
-    <hyperlink r:id="rId43" ref="X34"/>
-    <hyperlink r:id="rId44" ref="Y34"/>
-    <hyperlink r:id="rId45" ref="Z34"/>
-    <hyperlink r:id="rId46" ref="T38"/>
-    <hyperlink r:id="rId47" ref="U39"/>
-    <hyperlink r:id="rId48" ref="T41"/>
-    <hyperlink r:id="rId49" ref="T52"/>
-    <hyperlink r:id="rId50" ref="V53"/>
-    <hyperlink r:id="rId51" ref="U54"/>
-    <hyperlink r:id="rId52" ref="T55"/>
-    <hyperlink r:id="rId53" ref="U58"/>
-    <hyperlink r:id="rId54" ref="U59"/>
-    <hyperlink r:id="rId55" ref="U60"/>
-    <hyperlink r:id="rId56" ref="U61"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="U4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="V4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="U6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="U7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="V7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="T8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="U8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="T9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="U9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="V9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="X9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="U10" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="U11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="V11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="T12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="U12" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="T14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="U14" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="V14" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="U15" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="V15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="T16" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="T18" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="U18" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="V18" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="W18" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="T20" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="U20" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="T22" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="U22" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="U23" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="V23" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C24" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="U25" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="U27" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="U28" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="U29" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="U32" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="U33" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="U34" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="V34" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="X34" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="Y34" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="Z34" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="T38" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="U39" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="T41" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="T52" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="V53" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="U54" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="T55" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="U58" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="U59" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="U60" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="U61" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
   </hyperlinks>
-  <drawing r:id="rId57"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="6.13"/>
-    <col customWidth="1" min="8" max="8" width="16.5"/>
-    <col customWidth="1" min="10" max="10" width="20.75"/>
-    <col customWidth="1" min="13" max="13" width="18.5"/>
-    <col customWidth="1" min="15" max="15" width="19.63"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>394</v>
       </c>
@@ -4480,95 +4520,76 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>408</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>723</v>
+      </c>
+      <c r="C2">
+        <v>1954</v>
+      </c>
+      <c r="D2" t="s">
         <v>409</v>
       </c>
-      <c r="C2" s="1">
-        <v>1954.0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
         <v>410</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="M2" t="s">
         <v>411</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="S2" t="s">
         <v>412</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:32" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3" t="s">
+        <v>724</v>
+      </c>
+      <c r="C3">
+        <v>2008</v>
+      </c>
+      <c r="D3" t="s">
         <v>413</v>
       </c>
-      <c r="T2" s="3"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>414</v>
       </c>
-      <c r="C3" s="1">
-        <v>2008.0</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" t="s">
         <v>415</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" t="s">
         <v>416</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="M3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="M3" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="3"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>421</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>198</v>
@@ -4577,252 +4598,252 @@
         <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1"/>
+      <c r="S4" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="T4" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="R4" s="3"/>
-      <c r="S4" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="5">
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="R5" s="3"/>
-      <c r="S5" s="2" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="T5" s="3"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9" t="s">
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="7" t="s">
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="7" t="s">
+      <c r="B7" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="C7" s="1">
-        <v>2009.0</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="8">
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>453</v>
       </c>
       <c r="K8" s="1"/>
       <c r="M8" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="S8" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="Q8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>462</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>251</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="10">
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="C10" s="1">
-        <v>2020.0</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>470</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>159</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>32</v>
@@ -4831,110 +4852,110 @@
         <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="S11" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="P11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="C12" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="C12" s="1">
-        <v>2022.0</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>488</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="Q12" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="R12" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="Q12" s="6" t="s">
+      <c r="S12" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="S12" s="4" t="s">
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>498</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>140</v>
       </c>
       <c r="S13" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>502</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>21</v>
@@ -4943,21 +4964,21 @@
         <v>126</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C15" s="1">
-        <v>1977.0</v>
+        <v>1977</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>21</v>
@@ -4969,16 +4990,16 @@
         <v>340</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="T15" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="S15" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="16">
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>408</v>
       </c>
@@ -4987,10 +5008,10 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
@@ -5000,56 +5021,56 @@
         <v>140</v>
       </c>
       <c r="S16" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="S17" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="T17" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="S17" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="18">
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C18" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>198</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>340</v>
@@ -5058,18 +5079,18 @@
         <v>140</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C19" s="1">
-        <v>1982.0</v>
+        <v>1982</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>198</v>
@@ -5078,47 +5099,47 @@
         <v>21</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="S19" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="20">
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>533</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>535</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>198</v>
@@ -5127,54 +5148,92 @@
         <v>21</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>498</v>
+      </c>
+      <c r="B22" t="s">
+        <v>712</v>
+      </c>
+      <c r="C22" t="s">
+        <v>713</v>
+      </c>
+      <c r="D22" t="s">
+        <v>714</v>
+      </c>
+      <c r="E22" t="s">
+        <v>715</v>
+      </c>
+      <c r="F22" t="s">
+        <v>716</v>
+      </c>
+      <c r="G22" t="s">
+        <v>717</v>
+      </c>
+      <c r="J22" t="s">
+        <v>718</v>
+      </c>
+      <c r="P22" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>720</v>
+      </c>
+      <c r="S22" t="s">
+        <v>721</v>
+      </c>
+      <c r="T22" t="s">
+        <v>722</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="S2"/>
-    <hyperlink r:id="rId2" ref="S4"/>
-    <hyperlink r:id="rId3" ref="T4"/>
-    <hyperlink r:id="rId4" ref="S5"/>
-    <hyperlink r:id="rId5" ref="S8"/>
-    <hyperlink r:id="rId6" ref="S10"/>
-    <hyperlink r:id="rId7" ref="S11"/>
-    <hyperlink r:id="rId8" ref="R12"/>
-    <hyperlink r:id="rId9" ref="S12"/>
-    <hyperlink r:id="rId10" ref="T12"/>
-    <hyperlink r:id="rId11" ref="S13"/>
-    <hyperlink r:id="rId12" ref="S15"/>
-    <hyperlink r:id="rId13" ref="T15"/>
-    <hyperlink r:id="rId14" ref="S16"/>
-    <hyperlink r:id="rId15" ref="S17"/>
-    <hyperlink r:id="rId16" ref="T17"/>
-    <hyperlink r:id="rId17" ref="S18"/>
-    <hyperlink r:id="rId18" ref="S19"/>
+    <hyperlink ref="S4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="T4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="S5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="S8" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="S10" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="S11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="R12" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="S12" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="T12" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="S13" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="S15" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="T15" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="S16" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="S17" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="T17" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="S18" r:id="rId16" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="S19" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
   </hyperlinks>
-  <drawing r:id="rId19"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="6.25"/>
-    <col customWidth="1" min="7" max="7" width="17.88"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5183,40 +5242,40 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>546</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>549</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
@@ -5231,58 +5290,58 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1954</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1954.0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>553</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>558</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>560</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>209</v>
@@ -5290,175 +5349,175 @@
       <c r="I3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1998.0</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>564</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>566</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>159</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="1">
-        <v>2024.0</v>
+        <v>2024</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>571</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>573</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>121</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>584</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>586</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>588</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>179</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>589</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>591</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="s">
@@ -5467,67 +5526,67 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>596</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>598</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>179</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
@@ -5536,24 +5595,24 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="G11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
@@ -5562,12 +5621,12 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
@@ -5577,116 +5636,116 @@
         <v>245</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>608</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>609</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>610</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="S12" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>619</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>621</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="S13" s="3"/>
-    </row>
-    <row r="14">
+        <v>554</v>
+      </c>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2008</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="C14" s="1">
-        <v>2008.0</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="I14" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>629</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>631</v>
       </c>
       <c r="M14" s="1"/>
       <c r="O14" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="S14" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" s="2" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>632</v>
-      </c>
-      <c r="T14" s="3"/>
-      <c r="U14" s="2" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>634</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
@@ -5696,14 +5755,14 @@
         <v>327</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
@@ -5712,57 +5771,57 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>327</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>348</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>365</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>357</v>
@@ -5771,70 +5830,70 @@
         <v>141</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="H18" s="3"/>
+      <c r="H18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="R18" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="S18" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="U18" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="S18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>654</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>656</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>659</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>661</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>351</v>
@@ -5842,37 +5901,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="S2"/>
-    <hyperlink r:id="rId2" ref="S4"/>
-    <hyperlink r:id="rId3" ref="S5"/>
-    <hyperlink r:id="rId4" ref="S12"/>
-    <hyperlink r:id="rId5" ref="T12"/>
-    <hyperlink r:id="rId6" ref="S14"/>
-    <hyperlink r:id="rId7" ref="U14"/>
-    <hyperlink r:id="rId8" ref="R18"/>
-    <hyperlink r:id="rId9" ref="S18"/>
-    <hyperlink r:id="rId10" ref="U18"/>
-    <hyperlink r:id="rId11" ref="R19"/>
+    <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="S4" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="S5" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="S12" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="T12" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="S14" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="U14" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="R18" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="S18" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="U18" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="R19" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
   </hyperlinks>
-  <drawing r:id="rId12"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="15.63"/>
-    <col customWidth="1" min="20" max="20" width="33.38"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="20" max="20" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>394</v>
       </c>
@@ -5883,13 +5943,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>405</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -5916,16 +5976,16 @@
         <v>401</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>664</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>666</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>406</v>
@@ -5937,199 +5997,199 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>667</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="F2" s="5" t="s">
         <v>669</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>671</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
         <v>673</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="5" t="s">
         <v>674</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="7" t="s">
+      <c r="N2" s="5" t="s">
         <v>675</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="7" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="7" t="s">
+      <c r="S2" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="7" t="s">
+      <c r="T2" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="U2" s="6" t="s">
         <v>680</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="V2" s="6" t="s">
         <v>681</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="W2" s="6" t="s">
         <v>682</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="X2" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="Y2" s="6" t="s">
         <v>684</v>
       </c>
-      <c r="X2" s="11" t="s">
-        <v>685</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>686</v>
-      </c>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-    </row>
-    <row r="3">
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>408</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>689</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>691</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>99</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="V3" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="W3" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="V3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>701</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>707</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>709</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>278</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>710</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="V4" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="5">
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="V5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2"/>
-    <hyperlink r:id="rId2" ref="V2"/>
-    <hyperlink r:id="rId3" ref="W2"/>
-    <hyperlink r:id="rId4" ref="X2"/>
-    <hyperlink r:id="rId5" ref="Y2"/>
-    <hyperlink r:id="rId6" location="cite_note-11" ref="V3"/>
-    <hyperlink r:id="rId7" ref="W3"/>
-    <hyperlink r:id="rId8" ref="V4"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="V3" r:id="rId6" location="cite_note-11" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="W3" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="V4" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
   </hyperlinks>
-  <drawing r:id="rId9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Foundation Filed Cases, Related Cases, Not Litigated
</commit_message>
<xml_diff>
--- a/Cases in Film_Music_Arts - List Foundations.xlsx
+++ b/Cases in Film_Music_Arts - List Foundations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Actresses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB027B17-DBB3-4113-ACF7-94DBEB71A0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62D9936-12A9-4255-8725-FAB215D9B74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2214,10 +2214,10 @@
     <t>https://www.nytimes.com/2019/08/26/us/epstein-farmer-sisters-maxwell.html</t>
   </si>
   <si>
-    <t>Many-National, Hollywood</t>
-  </si>
-  <si>
     <t>Many- National, Hollywood, Arts</t>
+  </si>
+  <si>
+    <t>Many-National, Hollywood Social Circles</t>
   </si>
 </sst>
 </file>
@@ -4452,7 +4452,7 @@
   <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4525,7 +4525,7 @@
         <v>408</v>
       </c>
       <c r="B2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C2">
         <v>1954</v>
@@ -4557,7 +4557,7 @@
         <v>408</v>
       </c>
       <c r="B3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C3">
         <v>2008</v>

</xml_diff>

<commit_message>
Cases in Film, Music, Arts - Related Cases, Civil, Criminal, Others
</commit_message>
<xml_diff>
--- a/Cases in Film_Music_Arts - List Foundations.xlsx
+++ b/Cases in Film_Music_Arts - List Foundations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Actresses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D11634-2665-45C5-85A2-26369A207D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF2CEAC-DECE-49BE-988E-6D260DD731F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="1109">
   <si>
     <t>State</t>
   </si>
@@ -2959,9 +2959,6 @@
     <t>Medical, Exploitation, Conservatorship</t>
   </si>
   <si>
-    <t>Molly Bloom</t>
-  </si>
-  <si>
     <t>Social, High-Level Gambling, Hotels, Nightclubs, Olympic Athlete</t>
   </si>
   <si>
@@ -3317,6 +3314,42 @@
   </si>
   <si>
     <t>Sean Combs, RICO</t>
+  </si>
+  <si>
+    <t>Lou Pearlman</t>
+  </si>
+  <si>
+    <t>https://www.today.com/popculture/lou-pearlman-indicted-fraud-charges-1C9430730</t>
+  </si>
+  <si>
+    <t>FBI, Federal Authorities, Integra Bank</t>
+  </si>
+  <si>
+    <t>Investors seek justice</t>
+  </si>
+  <si>
+    <t>https://www.netflix.com/title/81476403</t>
+  </si>
+  <si>
+    <t>Implication Artists, TV Show, 315 million defrauded investors, 120 million to banks, 20 million to Integra Bank</t>
+  </si>
+  <si>
+    <t>1990s-2007</t>
+  </si>
+  <si>
+    <t>Music, Boy Bands, Airplane Charter, Real Estate, Model Scouting, Restaurants, Financial, N Sync, Backstreet Boys</t>
+  </si>
+  <si>
+    <t>Fraud, Fraudulent Documents, Fake Accounting Firm, Wire Fraud, Ponzi Scheme</t>
+  </si>
+  <si>
+    <t>Investors, Integra Bank N.A., Social Circles Artists</t>
+  </si>
+  <si>
+    <t>Molly Bloom, Potentially Others</t>
+  </si>
+  <si>
+    <t>Alexa Nikolas, Family</t>
   </si>
 </sst>
 </file>
@@ -3383,12 +3416,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3874,13 +3908,13 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D7" t="s">
         <v>1090</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1091</v>
       </c>
       <c r="G7" t="s">
         <v>358</v>
@@ -3892,54 +3926,54 @@
         <v>360</v>
       </c>
       <c r="R7" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="S7" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="T7" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B8">
         <v>2024</v>
       </c>
       <c r="C8" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D8" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1079</v>
+      </c>
+      <c r="I8" t="s">
         <v>1085</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1079</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1080</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1086</v>
       </c>
       <c r="J8" t="s">
         <v>112</v>
       </c>
       <c r="K8" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="R8" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="T8" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="U8" t="s">
+        <v>1081</v>
+      </c>
+      <c r="V8" t="s">
         <v>1082</v>
-      </c>
-      <c r="V8" t="s">
-        <v>1083</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -4458,7 +4492,7 @@
         <v>2015</v>
       </c>
       <c r="C26" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D26" t="s">
         <v>194</v>
@@ -4655,7 +4689,7 @@
         <v>233</v>
       </c>
       <c r="C33" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D33" t="s">
         <v>234</v>
@@ -5602,7 +5636,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T33"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -5735,13 +5769,13 @@
         <v>413</v>
       </c>
       <c r="B4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C4" t="s">
         <v>414</v>
       </c>
       <c r="D4" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -5770,7 +5804,7 @@
         <v>889</v>
       </c>
       <c r="B5" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C5" t="s">
         <v>837</v>
@@ -5788,7 +5822,7 @@
         <v>838</v>
       </c>
       <c r="J5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="K5" t="s">
         <v>850</v>
@@ -5797,10 +5831,10 @@
         <v>839</v>
       </c>
       <c r="P5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="Q5" t="s">
         <v>1028</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>1029</v>
       </c>
       <c r="S5" t="s">
         <v>840</v>
@@ -5884,7 +5918,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B8" t="s">
         <v>969</v>
@@ -5893,19 +5927,19 @@
         <v>824</v>
       </c>
       <c r="D8" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="J8" t="s">
         <v>971</v>
       </c>
       <c r="K8" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="P8" t="s">
         <v>972</v>
@@ -5922,7 +5956,7 @@
         <v>432</v>
       </c>
       <c r="B9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C9">
         <v>2009</v>
@@ -5957,46 +5991,46 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B10" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C10" t="s">
         <v>438</v>
       </c>
       <c r="D10" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E10" t="s">
         <v>1001</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1002</v>
       </c>
       <c r="F10" t="s">
         <v>410</v>
       </c>
       <c r="G10" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I10" t="s">
         <v>1003</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>1004</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>1005</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>1006</v>
       </c>
-      <c r="M10" t="s">
+      <c r="P10" t="s">
         <v>1007</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>1008</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>1009</v>
-      </c>
-      <c r="S10" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -6022,7 +6056,7 @@
         <v>687</v>
       </c>
       <c r="J11" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P11" t="s">
         <v>688</v>
@@ -6063,10 +6097,10 @@
         <v>895</v>
       </c>
       <c r="K12" t="s">
+        <v>1024</v>
+      </c>
+      <c r="P12" t="s">
         <v>1025</v>
-      </c>
-      <c r="P12" t="s">
-        <v>1026</v>
       </c>
       <c r="S12" t="s">
         <v>731</v>
@@ -6103,16 +6137,16 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B14" t="s">
         <v>1031</v>
       </c>
-      <c r="B14" t="s">
-        <v>1032</v>
-      </c>
       <c r="C14" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D14" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
@@ -6121,22 +6155,22 @@
         <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="I14" t="s">
+        <v>1032</v>
+      </c>
+      <c r="J14" t="s">
         <v>1033</v>
       </c>
-      <c r="J14" t="s">
+      <c r="P14" t="s">
         <v>1034</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>1035</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" s="1" t="s">
         <v>1036</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -6144,7 +6178,7 @@
         <v>404</v>
       </c>
       <c r="B15" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C15" t="s">
         <v>887</v>
@@ -6176,7 +6210,7 @@
         <v>404</v>
       </c>
       <c r="B16" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C16" t="s">
         <v>438</v>
@@ -6264,7 +6298,7 @@
         <v>32</v>
       </c>
       <c r="G18" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="J18" t="s">
         <v>464</v>
@@ -6339,35 +6373,35 @@
       <c r="A20" t="s">
         <v>911</v>
       </c>
-      <c r="B20" t="s">
-        <v>978</v>
+      <c r="B20" s="4" t="s">
+        <v>1107</v>
       </c>
       <c r="C20">
         <v>2014</v>
       </c>
       <c r="D20" t="s">
+        <v>978</v>
+      </c>
+      <c r="E20" t="s">
         <v>979</v>
-      </c>
-      <c r="E20" t="s">
-        <v>980</v>
       </c>
       <c r="F20" t="s">
         <v>410</v>
       </c>
       <c r="G20" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="J20" t="s">
+        <v>980</v>
+      </c>
+      <c r="K20" t="s">
         <v>981</v>
       </c>
-      <c r="K20" t="s">
+      <c r="P20" t="s">
         <v>982</v>
       </c>
-      <c r="P20" t="s">
+      <c r="S20" t="s">
         <v>983</v>
-      </c>
-      <c r="S20" t="s">
-        <v>984</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
@@ -6714,14 +6748,14 @@
       <c r="A32" t="s">
         <v>606</v>
       </c>
-      <c r="B32" t="s">
-        <v>325</v>
+      <c r="B32" s="4" t="s">
+        <v>1108</v>
       </c>
       <c r="C32" t="s">
+        <v>985</v>
+      </c>
+      <c r="D32" t="s">
         <v>986</v>
-      </c>
-      <c r="D32" t="s">
-        <v>987</v>
       </c>
       <c r="E32" t="s">
         <v>21</v>
@@ -6730,7 +6764,7 @@
         <v>605</v>
       </c>
       <c r="J32" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="K32" t="s">
         <v>241</v>
@@ -6739,7 +6773,7 @@
         <v>141</v>
       </c>
       <c r="P32" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="S32" t="s">
         <v>760</v>
@@ -6750,42 +6784,81 @@
         <v>404</v>
       </c>
       <c r="B33" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C33" t="s">
         <v>1013</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>1014</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>1015</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>1016</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>1017</v>
       </c>
-      <c r="H33" t="s">
+      <c r="J33" t="s">
         <v>1018</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>1019</v>
       </c>
-      <c r="K33" t="s">
+      <c r="P33" t="s">
         <v>1020</v>
       </c>
-      <c r="P33" t="s">
+      <c r="S33" t="s">
         <v>1021</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>1022</v>
       </c>
-      <c r="T33" t="s">
-        <v>1023</v>
+    </row>
+    <row r="34" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="S34" s="5" t="s">
+        <v>1098</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>1101</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="S14" r:id="rId1" xr:uid="{07E42739-3C6B-4490-84B1-CD88824F1D3B}"/>
+    <hyperlink ref="S34" r:id="rId2" xr:uid="{73CF35C7-B40E-48BA-95DD-51FC2F0FB138}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6872,7 +6945,7 @@
         <v>1954</v>
       </c>
       <c r="D2" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E2" t="s">
         <v>538</v>
@@ -6881,7 +6954,7 @@
         <v>539</v>
       </c>
       <c r="G2" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="I2" t="s">
         <v>540</v>
@@ -7027,7 +7100,7 @@
         <v>694</v>
       </c>
       <c r="D6" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E6" t="s">
         <v>544</v>
@@ -7377,7 +7450,7 @@
         <v>567</v>
       </c>
       <c r="D16" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E16" t="s">
         <v>803</v>
@@ -7415,7 +7488,7 @@
         <v>572</v>
       </c>
       <c r="D17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E17" t="s">
         <v>730</v>
@@ -7709,7 +7782,7 @@
         <v>2008</v>
       </c>
       <c r="D26" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E26" t="s">
         <v>598</v>
@@ -8246,7 +8319,7 @@
         <v>660</v>
       </c>
       <c r="I3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J3" t="s">
         <v>660</v>
@@ -8255,7 +8328,7 @@
         <v>661</v>
       </c>
       <c r="N3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="P3" t="s">
         <v>662</v>
@@ -8284,46 +8357,46 @@
         <v>404</v>
       </c>
       <c r="B4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1048</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1050</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="T4" t="s">
         <v>1073</v>
       </c>
-      <c r="C4" t="s">
-        <v>1065</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>1078</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1071</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1072</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>1066</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1048</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1049</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1050</v>
-      </c>
-      <c r="R4" t="s">
-        <v>1051</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="V4" s="3" t="s">
         <v>1052</v>
-      </c>
-      <c r="T4" t="s">
-        <v>1074</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>1053</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
@@ -8375,55 +8448,55 @@
         <v>404</v>
       </c>
       <c r="B6" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D6" t="s">
         <v>1069</v>
       </c>
-      <c r="C6" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1070</v>
-      </c>
       <c r="E6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1058</v>
+      </c>
+      <c r="G6" t="s">
         <v>1054</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
+        <v>1055</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1076</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1056</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1057</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1063</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1062</v>
+      </c>
+      <c r="S6" t="s">
+        <v>1061</v>
+      </c>
+      <c r="T6" t="s">
+        <v>1060</v>
+      </c>
+      <c r="U6" s="3" t="s">
         <v>1059</v>
       </c>
-      <c r="G6" t="s">
-        <v>1055</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1056</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1077</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1057</v>
-      </c>
-      <c r="M6" t="s">
-        <v>1058</v>
-      </c>
-      <c r="N6" t="s">
-        <v>1068</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>1064</v>
-      </c>
-      <c r="R6" t="s">
-        <v>1063</v>
-      </c>
-      <c r="S6" t="s">
-        <v>1062</v>
-      </c>
-      <c r="T6" t="s">
-        <v>1061</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>1060</v>
-      </c>
       <c r="V6" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>